<commit_message>
Base de datos transporte
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Refineries_Flex.xlsx
+++ b/SuppXLS/Scen_Refineries_Flex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8499E81-AD38-413F-A561-6223181C0F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF23BE1-077B-483E-95DA-B17B68A33ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REF2-LO" sheetId="5" r:id="rId1"/>
@@ -838,8 +838,8 @@
   </sheetPr>
   <dimension ref="D4:AK72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:K9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6587,8 +6587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00905DE-6CE8-4F5B-9115-2E641D5266FC}">
   <dimension ref="D4:AL63"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6735,7 +6735,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="30">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="J9" s="26">
         <v>1.7999999999999999E-2</v>
@@ -6804,7 +6804,7 @@
       </c>
       <c r="I12">
         <f>+SUM(I6:I11)</f>
-        <v>0.77500000000000002</v>
+        <v>0.78400000000000014</v>
       </c>
       <c r="J12" s="27">
         <f t="shared" ref="J12:K12" si="0">+SUM(J6:J11)</f>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="U22" s="26">
         <f>+SUM(J22:J27)</f>
-        <v>0.77500000000000002</v>
+        <v>0.78400000000000014</v>
       </c>
       <c r="AA22" s="26"/>
       <c r="AB22" s="26"/>
@@ -7222,7 +7222,7 @@
         <v>26</v>
       </c>
       <c r="J25" s="26">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="L25" t="s">
         <v>25</v>
@@ -7309,7 +7309,7 @@
       </c>
       <c r="U28">
         <f>+SUM(J28:J33)</f>
-        <v>0.77500000000000002</v>
+        <v>0.78400000000000014</v>
       </c>
     </row>
     <row r="29" spans="4:36" x14ac:dyDescent="0.25">
@@ -7388,7 +7388,7 @@
       </c>
       <c r="I31" s="16"/>
       <c r="J31" s="22">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="K31" s="16"/>
       <c r="L31" s="16" t="s">
@@ -7487,7 +7487,7 @@
       </c>
       <c r="U34">
         <f>+SUM(J34:J39)</f>
-        <v>0.77500000000000002</v>
+        <v>0.78400000000000014</v>
       </c>
     </row>
     <row r="35" spans="4:38" x14ac:dyDescent="0.25">
@@ -7550,7 +7550,7 @@
         <v>26</v>
       </c>
       <c r="J37" s="26">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="L37" t="s">
         <v>25</v>
@@ -7637,7 +7637,7 @@
       </c>
       <c r="U40">
         <f>+SUM(J40:J45)</f>
-        <v>0.77500000000000002</v>
+        <v>0.78400000000000014</v>
       </c>
       <c r="AB40" s="26"/>
       <c r="AC40" s="26"/>
@@ -7746,7 +7746,7 @@
       </c>
       <c r="I43" s="16"/>
       <c r="J43" s="22">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16" t="s">
@@ -7876,7 +7876,7 @@
       </c>
       <c r="U46">
         <f>+SUM(J46:J51)</f>
-        <v>0.77500000000000002</v>
+        <v>0.78400000000000014</v>
       </c>
     </row>
     <row r="47" spans="4:38" x14ac:dyDescent="0.25">
@@ -7939,7 +7939,7 @@
         <v>26</v>
       </c>
       <c r="J49" s="26">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="L49" t="s">
         <v>25</v>
@@ -8026,7 +8026,7 @@
       </c>
       <c r="U52">
         <f>+SUM(J52:J57)</f>
-        <v>0.77500000000000002</v>
+        <v>0.78400000000000014</v>
       </c>
     </row>
     <row r="53" spans="4:21" x14ac:dyDescent="0.25">
@@ -8105,7 +8105,7 @@
       </c>
       <c r="I55" s="16"/>
       <c r="J55" s="22">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="K55" s="16"/>
       <c r="L55" s="16" t="s">
@@ -8204,7 +8204,7 @@
       </c>
       <c r="U58">
         <f>+SUM(J58:J63)</f>
-        <v>0.77500000000000002</v>
+        <v>0.78400000000000014</v>
       </c>
     </row>
     <row r="59" spans="4:21" x14ac:dyDescent="0.25">
@@ -8267,7 +8267,7 @@
         <v>26</v>
       </c>
       <c r="J61" s="26">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="L61" t="s">
         <v>25</v>

</xml_diff>